<commit_message>
LXX project and data visualisations
</commit_message>
<xml_diff>
--- a/6_conferences_notebooks/Hebrew_Bible_Septuagint_Project/data/greek_verbs/δυσμή.xlsx
+++ b/6_conferences_notebooks/Hebrew_Bible_Septuagint_Project/data/greek_verbs/δυσμή.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -527,6 +527,43 @@
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr"/>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>40982_lxx</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>40982_mt</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>ἐὰν δὲ ἐνεχύρασμα ἐνεχυράσῃς τὸ ἱμάτιον τοῦ πλησίον, πρὸ δυσμῶν ἡλίου ἀποδώσεις αὐτῷ ·</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>(22, 25)</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>&gt;M XBL TXBL FLMT R&lt;K &lt;D B&gt; H CMC TCJBNW LW</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>no complement</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>